<commit_message>
Fetch value from excel
Completed fetching value from excel and write into the dictionary
</commit_message>
<xml_diff>
--- a/Referral/localization.xlsx
+++ b/Referral/localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\320052425\Desktop\Rest_API_Automation_Python\Referral\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177EF79F-A8CC-4752-B212-2B5C7ABAA58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD09572-2C01-40DD-A55B-D840742380B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CB8B5040-33BA-4E9B-B8D1-883A405B4FB4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>HEADER_TEXT</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>Recomandă o prietenă și oferă-i posibilitatea de a achiziționa un Philips Lumea la reducere!</t>
-  </si>
-  <si>
-    <t>KKD</t>
   </si>
 </sst>
 </file>
@@ -625,7 +622,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>37</v>

</xml_diff>